<commit_message>
New Excel and PDF files with updated data
</commit_message>
<xml_diff>
--- a/weather_data_lat47.37_lon8.55.xlsx
+++ b/weather_data_lat47.37_lon8.55.xlsx
@@ -453,505 +453,505 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-08-26T09:00</t>
+          <t>2025-08-27T08:00</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>21.6</v>
       </c>
       <c r="C2" t="n">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-08-26T10:00</t>
+          <t>2025-08-27T09:00</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24.1</v>
+        <v>23.1</v>
       </c>
       <c r="C3" t="n">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-08-26T11:00</t>
+          <t>2025-08-27T10:00</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25.3</v>
+        <v>24.5</v>
       </c>
       <c r="C4" t="n">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-08-26T12:00</t>
+          <t>2025-08-27T11:00</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="C5" t="n">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-08-26T13:00</t>
+          <t>2025-08-27T12:00</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27.2</v>
+        <v>26.7</v>
       </c>
       <c r="C6" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-08-26T14:00</t>
+          <t>2025-08-27T13:00</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>27.9</v>
+        <v>26.9</v>
       </c>
       <c r="C7" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-08-26T15:00</t>
+          <t>2025-08-27T14:00</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>28.2</v>
+        <v>26.2</v>
       </c>
       <c r="C8" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-08-26T16:00</t>
+          <t>2025-08-27T15:00</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>27.9</v>
+        <v>24.2</v>
       </c>
       <c r="C9" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-08-26T17:00</t>
+          <t>2025-08-27T16:00</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26.8</v>
+        <v>23</v>
       </c>
       <c r="C10" t="n">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-08-26T18:00</t>
+          <t>2025-08-27T17:00</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>24</v>
+        <v>22.5</v>
       </c>
       <c r="C11" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-08-26T19:00</t>
+          <t>2025-08-27T18:00</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>22.5</v>
+        <v>20.8</v>
       </c>
       <c r="C12" t="n">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-08-26T20:00</t>
+          <t>2025-08-27T19:00</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>22.2</v>
+        <v>20.3</v>
       </c>
       <c r="C13" t="n">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-08-26T21:00</t>
+          <t>2025-08-27T20:00</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>21</v>
+        <v>19.8</v>
       </c>
       <c r="C14" t="n">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-08-26T22:00</t>
+          <t>2025-08-27T21:00</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>19.3</v>
       </c>
       <c r="C15" t="n">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-08-26T23:00</t>
+          <t>2025-08-27T22:00</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>19.4</v>
+        <v>18.9</v>
       </c>
       <c r="C16" t="n">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-08-27T00:00</t>
+          <t>2025-08-27T23:00</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>18.8</v>
+        <v>18.6</v>
       </c>
       <c r="C17" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-08-27T01:00</t>
+          <t>2025-08-28T00:00</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>18.6</v>
+        <v>18</v>
       </c>
       <c r="C18" t="n">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-08-27T02:00</t>
+          <t>2025-08-28T01:00</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>18.7</v>
+        <v>18.3</v>
       </c>
       <c r="C19" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-08-27T03:00</t>
+          <t>2025-08-28T02:00</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>18.8</v>
+        <v>17.9</v>
       </c>
       <c r="C20" t="n">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-08-27T04:00</t>
+          <t>2025-08-28T03:00</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>19</v>
+        <v>17.8</v>
       </c>
       <c r="C21" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-08-27T05:00</t>
+          <t>2025-08-28T04:00</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>19.1</v>
+        <v>17.9</v>
       </c>
       <c r="C22" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-08-27T06:00</t>
+          <t>2025-08-28T05:00</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>19.7</v>
+        <v>17.4</v>
       </c>
       <c r="C23" t="n">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-08-27T07:00</t>
+          <t>2025-08-28T06:00</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>20.7</v>
+        <v>17.2</v>
       </c>
       <c r="C24" t="n">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-08-27T08:00</t>
+          <t>2025-08-28T07:00</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>21.6</v>
+        <v>17.3</v>
       </c>
       <c r="C25" t="n">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-08-27T09:00</t>
+          <t>2025-08-28T08:00</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>23.1</v>
+        <v>17.5</v>
       </c>
       <c r="C26" t="n">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-08-27T10:00</t>
+          <t>2025-08-28T09:00</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>24.5</v>
+        <v>17.4</v>
       </c>
       <c r="C27" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-08-27T11:00</t>
+          <t>2025-08-28T10:00</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>26</v>
+        <v>17.4</v>
       </c>
       <c r="C28" t="n">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-08-27T12:00</t>
+          <t>2025-08-28T11:00</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>26.7</v>
+        <v>18.1</v>
       </c>
       <c r="C29" t="n">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-08-27T13:00</t>
+          <t>2025-08-28T12:00</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>26.9</v>
+        <v>18.5</v>
       </c>
       <c r="C30" t="n">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-08-27T14:00</t>
+          <t>2025-08-28T13:00</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>26.2</v>
+        <v>18.6</v>
       </c>
       <c r="C31" t="n">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-08-27T15:00</t>
+          <t>2025-08-28T14:00</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>24.2</v>
+        <v>18.7</v>
       </c>
       <c r="C32" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-08-27T16:00</t>
+          <t>2025-08-28T15:00</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>23</v>
+        <v>18.6</v>
       </c>
       <c r="C33" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-08-27T17:00</t>
+          <t>2025-08-28T16:00</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>22.5</v>
+        <v>18.6</v>
       </c>
       <c r="C34" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-08-27T18:00</t>
+          <t>2025-08-28T17:00</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>20.8</v>
+        <v>18.4</v>
       </c>
       <c r="C35" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-08-27T19:00</t>
+          <t>2025-08-28T18:00</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>20.3</v>
+        <v>18.5</v>
       </c>
       <c r="C36" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-08-27T20:00</t>
+          <t>2025-08-28T19:00</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>19.8</v>
+        <v>17.9</v>
       </c>
       <c r="C37" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-08-27T21:00</t>
+          <t>2025-08-28T20:00</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>19.3</v>
+        <v>17.2</v>
       </c>
       <c r="C38" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-08-27T22:00</t>
+          <t>2025-08-28T21:00</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>18.9</v>
+        <v>17.2</v>
       </c>
       <c r="C39" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-08-27T23:00</t>
+          <t>2025-08-28T22:00</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>18.6</v>
+        <v>16.9</v>
       </c>
       <c r="C40" t="n">
         <v>92</v>
@@ -960,118 +960,118 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-08-28T00:00</t>
+          <t>2025-08-28T23:00</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>18</v>
+        <v>16.7</v>
       </c>
       <c r="C41" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-08-28T01:00</t>
+          <t>2025-08-29T00:00</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>18.3</v>
+        <v>15.5</v>
       </c>
       <c r="C42" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-08-28T02:00</t>
+          <t>2025-08-29T01:00</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>17.9</v>
+        <v>15</v>
       </c>
       <c r="C43" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-08-28T03:00</t>
+          <t>2025-08-29T02:00</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>17.8</v>
+        <v>14.8</v>
       </c>
       <c r="C44" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-08-28T04:00</t>
+          <t>2025-08-29T03:00</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>17.9</v>
+        <v>14.6</v>
       </c>
       <c r="C45" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-08-28T05:00</t>
+          <t>2025-08-29T04:00</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>17.4</v>
+        <v>14.5</v>
       </c>
       <c r="C46" t="n">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-08-28T06:00</t>
+          <t>2025-08-29T05:00</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>17.2</v>
+        <v>14.3</v>
       </c>
       <c r="C47" t="n">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-08-28T07:00</t>
+          <t>2025-08-29T06:00</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>17.3</v>
+        <v>15</v>
       </c>
       <c r="C48" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-08-28T08:00</t>
+          <t>2025-08-29T07:00</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>17.5</v>
+        <v>15.9</v>
       </c>
       <c r="C49" t="n">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>